<commit_message>
Fixing errors and adding data provider
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/invalid_login_data.xlsx
+++ b/src/main/resources/Data/invalid_login_data.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9570"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9570"/>
   </bookViews>
   <sheets>
-    <sheet name="loginDataSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidLoginDataSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -43,48 +43,6 @@
   </si>
   <si>
     <t>TVHt389V2lfW</t>
-  </si>
-  <si>
-    <t>nfeatherbie3</t>
-  </si>
-  <si>
-    <t>loe1WLBvx2</t>
-  </si>
-  <si>
-    <t>klyston4</t>
-  </si>
-  <si>
-    <t>dEfjpUu</t>
-  </si>
-  <si>
-    <t>jkhomin5</t>
-  </si>
-  <si>
-    <t>tqNlTitlxY</t>
-  </si>
-  <si>
-    <t>dmcgorley6</t>
-  </si>
-  <si>
-    <t>xywDqYbKpWo</t>
-  </si>
-  <si>
-    <t>pbellon7</t>
-  </si>
-  <si>
-    <t>ECdyYc79oe</t>
-  </si>
-  <si>
-    <t>kbromilow8</t>
-  </si>
-  <si>
-    <t>XiuMy7wpe</t>
-  </si>
-  <si>
-    <t>gspellacy9</t>
-  </si>
-  <si>
-    <t>D38l4XZ1vtgq</t>
   </si>
 </sst>
 </file>
@@ -400,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -444,62 +402,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>